<commit_message>
Modified Success Trend API
</commit_message>
<xml_diff>
--- a/QUARK-API/quarkapp/result_2.xlsx
+++ b/QUARK-API/quarkapp/result_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EAinfoBiz\Downloads\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\QUARK-API\QUARK-API\quarkapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCB387D-CEA6-4584-9B1A-E623177BE92B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE0845C-CFE6-4F70-B679-F93227506DB9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Transformed by JSON-CSV.COM" sheetId="2" r:id="rId1"/>
@@ -403,10 +403,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -718,71 +718,71 @@
   <dimension ref="A1:Q117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="S101" sqref="S101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="3"/>
       <c r="D1" s="1" t="s">
         <v>89</v>
       </c>
       <c r="E1" s="1"/>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="3"/>
       <c r="D2" s="1" t="s">
         <v>93</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>94</v>
       </c>
@@ -805,7 +805,7 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -858,7 +858,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -905,7 +905,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -934,7 +934,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -963,7 +963,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -992,7 +992,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1441,7 +1441,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -1517,7 +1517,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>27</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>28</v>
       </c>
@@ -1832,7 +1832,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>29</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>30</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>31</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>32</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>33</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>34</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>35</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>36</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>37</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>38</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>39</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>40</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>41</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>42</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>43</v>
       </c>
@@ -2447,7 +2447,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>44</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>45</v>
       </c>
@@ -2541,7 +2541,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>46</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>47</v>
       </c>
@@ -2635,7 +2635,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>48</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>49</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>50</v>
       </c>
@@ -2776,7 +2776,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>51</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>52</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>53</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>54</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>55</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>56</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>57</v>
       </c>
@@ -3105,7 +3105,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>58</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>59</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>60</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>61</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>62</v>
       </c>
@@ -3340,7 +3340,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>63</v>
       </c>
@@ -3387,7 +3387,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>64</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>65</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>66</v>
       </c>
@@ -3528,7 +3528,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>67</v>
       </c>
@@ -3575,7 +3575,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>68</v>
       </c>
@@ -3622,7 +3622,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>69</v>
       </c>
@@ -3669,7 +3669,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>70</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>71</v>
       </c>
@@ -3763,7 +3763,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>72</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>73</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>74</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>75</v>
       </c>
@@ -3951,7 +3951,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>76</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>77</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>78</v>
       </c>
@@ -4092,7 +4092,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>79</v>
       </c>
@@ -4139,7 +4139,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>80</v>
       </c>
@@ -4186,7 +4186,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>81</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>82</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>83</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>84</v>
       </c>
@@ -4374,7 +4374,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>85</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>86</v>
       </c>
@@ -4450,7 +4450,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>87</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>88</v>
       </c>
@@ -4544,7 +4544,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>89</v>
       </c>
@@ -4573,7 +4573,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>90</v>
       </c>
@@ -4602,7 +4602,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>91</v>
       </c>
@@ -4631,7 +4631,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>92</v>
       </c>
@@ -4660,7 +4660,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>93</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>94</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>95</v>
       </c>
@@ -4747,7 +4747,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>96</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>97</v>
       </c>
@@ -4823,7 +4823,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>98</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>99</v>
       </c>
@@ -4899,7 +4899,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>100</v>
       </c>
@@ -4946,7 +4946,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>101</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>102</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>103</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>104</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>105</v>
       </c>
@@ -5181,7 +5181,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>106</v>
       </c>
@@ -5228,7 +5228,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>107</v>
       </c>
@@ -5275,7 +5275,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>108</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>109</v>
       </c>
@@ -5369,7 +5369,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>110</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>111</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>112</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>113</v>
       </c>

</xml_diff>